<commit_message>
LED Control test 1
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4480" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4651" uniqueCount="115">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -356,6 +356,12 @@
   </si>
   <si>
     <t xml:space="preserve">Reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED</t>
   </si>
 </sst>
 </file>
@@ -1931,7 +1937,23 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="2:10"/>
+    <row r="10" spans="2:10">
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F10" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="11"/>
     <row r="12"/>
     <row r="13" spans="2:10"/>

</xml_diff>

<commit_message>
Clean project, update gitignore
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4765" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4936" uniqueCount="118">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t xml:space="preserve">Toggle Button (ajam text)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle Button (ajamtext)</t>
   </si>
 </sst>
 </file>
@@ -1903,7 +1906,7 @@
         <v>62</v>
       </c>
       <c r="E7" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F7" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Demo version to be uploaded
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4936" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6205" uniqueCount="126">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -371,6 +371,30 @@
   </si>
   <si>
     <t xml:space="preserve">Toggle Button (ajamtext)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toogle LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orange </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orange Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tLED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle LED</t>
   </si>
 </sst>
 </file>
@@ -1897,16 +1921,16 @@
     </row>
     <row r="7" spans="2:10">
       <c r="B7" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
         <v>76</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="F7" t="s">
         <v>59</v>
@@ -1914,16 +1938,16 @@
     </row>
     <row r="8" spans="2:10">
       <c r="B8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D8" t="s">
         <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="F8" t="s">
         <v>59</v>
@@ -1931,38 +1955,22 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D9" t="s">
         <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="F9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
-      <c r="B10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" t="s">
-        <v>114</v>
-      </c>
-      <c r="F10" t="s">
-        <v>59</v>
-      </c>
-    </row>
+    <row r="10" spans="2:10"/>
     <row r="11"/>
     <row r="12"/>
     <row r="13" spans="2:10"/>

</xml_diff>

<commit_message>
LWIP project files compiled, added GUI interface for TCP send, netcomm created, not yet transmitting data
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6205" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6319" uniqueCount="127">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -395,6 +395,9 @@
   </si>
   <si>
     <t xml:space="preserve">Toggle LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send TCP</t>
   </si>
 </sst>
 </file>
@@ -1970,7 +1973,23 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="2:10"/>
+    <row r="10" spans="2:10">
+      <c r="B10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="11"/>
     <row r="12"/>
     <row r="13" spans="2:10"/>

</xml_diff>

<commit_message>
Added log and dump features, both GUI and HAL
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6319" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6727" uniqueCount="133">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -398,6 +398,24 @@
   </si>
   <si>
     <t xml:space="preserve">Send TCP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dump Log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log Data</t>
   </si>
 </sst>
 </file>
@@ -1990,8 +2008,40 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11"/>
-    <row r="12"/>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" t="s">
+        <v>130</v>
+      </c>
+      <c r="F12" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="13" spans="2:10"/>
     <row r="14" spans="2:10"/>
     <row r="15" spans="2:10"/>

</xml_diff>

<commit_message>
Added new screens to split content
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6727" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6946" uniqueCount="134">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -416,6 +416,9 @@
   </si>
   <si>
     <t xml:space="preserve">Log Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
   </si>
 </sst>
 </file>
@@ -1976,7 +1979,7 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="C9" t="s">
         <v>76</v>
@@ -1985,7 +1988,7 @@
         <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F9" t="s">
         <v>59</v>
@@ -1993,7 +1996,7 @@
     </row>
     <row r="10" spans="2:10">
       <c r="B10" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
         <v>76</v>
@@ -2002,7 +2005,7 @@
         <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="F10" t="s">
         <v>59</v>
@@ -2010,7 +2013,7 @@
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C11" t="s">
         <v>76</v>
@@ -2019,7 +2022,7 @@
         <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F11" t="s">
         <v>59</v>
@@ -2027,7 +2030,7 @@
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C12" t="s">
         <v>76</v>
@@ -2036,7 +2039,7 @@
         <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F12" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Added Network IP Address to GUI
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9052" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17947" uniqueCount="191">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -485,6 +485,111 @@
   </si>
   <si>
     <t xml:space="preserve">Random</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192.168.0.17&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ipAddrText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Address Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Address 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ip_address&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP_Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x20-0x7E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,a-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255.255.255.255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arial.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0123456789.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB-ALIGNMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB-TYPOGRAPHY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB-DIRECTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2.3.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ip_&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ipaddress&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_00</t>
   </si>
 </sst>
 </file>
@@ -1812,6 +1917,28 @@
       <c r="O6" s="11"/>
     </row>
     <row r="7" spans="2:15">
+      <c r="B7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>186</v>
+      </c>
+      <c r="G7" t="s">
+        <v>167</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7"/>
       <c r="K7" s="8" t="s">
         <v>15</v>
       </c>
@@ -1829,6 +1956,7 @@
       </c>
     </row>
     <row r="8" spans="2:15">
+      <c r="I8"/>
       <c r="K8" s="8" t="s">
         <v>16</v>
       </c>
@@ -1957,6 +2085,12 @@
       <c r="F3" t="s">
         <v>57</v>
       </c>
+      <c r="G3" t="s">
+        <v>181</v>
+      </c>
+      <c r="H3" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="4" spans="2:10" ht="15" customHeight="1">
       <c r="B4" t="s">
@@ -1977,16 +2111,16 @@
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1">
       <c r="B5" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="F5" t="s">
         <v>59</v>
@@ -1994,16 +2128,16 @@
     </row>
     <row r="6" spans="2:10">
       <c r="B6" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
         <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="F6" t="s">
         <v>59</v>
@@ -2011,7 +2145,7 @@
     </row>
     <row r="7" spans="2:10">
       <c r="B7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
         <v>76</v>
@@ -2020,7 +2154,7 @@
         <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F7" t="s">
         <v>59</v>
@@ -2028,7 +2162,7 @@
     </row>
     <row r="8" spans="2:10">
       <c r="B8" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="C8" t="s">
         <v>76</v>
@@ -2037,7 +2171,7 @@
         <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F8" t="s">
         <v>59</v>
@@ -2045,7 +2179,7 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
         <v>76</v>
@@ -2054,7 +2188,7 @@
         <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F9" t="s">
         <v>59</v>
@@ -2062,7 +2196,7 @@
     </row>
     <row r="10" spans="2:10">
       <c r="B10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C10" t="s">
         <v>76</v>
@@ -2071,7 +2205,7 @@
         <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="F10" t="s">
         <v>59</v>
@@ -2079,7 +2213,7 @@
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C11" t="s">
         <v>76</v>
@@ -2088,7 +2222,7 @@
         <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F11" t="s">
         <v>59</v>
@@ -2096,7 +2230,7 @@
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C12" t="s">
         <v>76</v>
@@ -2105,7 +2239,7 @@
         <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="F12" t="s">
         <v>59</v>
@@ -2113,16 +2247,16 @@
     </row>
     <row r="13" spans="2:10">
       <c r="B13" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>137</v>
+        <v>95</v>
       </c>
       <c r="F13" t="s">
         <v>59</v>
@@ -2130,16 +2264,16 @@
     </row>
     <row r="14" spans="2:10">
       <c r="B14" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
-        <v>95</v>
+        <v>155</v>
       </c>
       <c r="F14" t="s">
         <v>59</v>
@@ -2147,7 +2281,7 @@
     </row>
     <row r="15" spans="2:10">
       <c r="B15" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C15" t="s">
         <v>76</v>
@@ -2156,7 +2290,7 @@
         <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="F15" t="s">
         <v>59</v>
@@ -2164,16 +2298,16 @@
     </row>
     <row r="16" spans="2:10">
       <c r="B16" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C16" t="s">
         <v>76</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>144</v>
       </c>
       <c r="E16" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="F16" t="s">
         <v>59</v>
@@ -2181,16 +2315,16 @@
     </row>
     <row r="17" spans="4:4">
       <c r="B17" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="C17" t="s">
         <v>76</v>
       </c>
       <c r="D17" t="s">
-        <v>144</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="F17" t="s">
         <v>59</v>
@@ -2198,16 +2332,16 @@
     </row>
     <row r="18" spans="4:4">
       <c r="B18" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
         <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="F18" t="s">
         <v>59</v>
@@ -2215,24 +2349,30 @@
     </row>
     <row r="19" spans="4:4">
       <c r="B19" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>169</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E19" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="F19" t="s">
         <v>59</v>
       </c>
+      <c r="G19" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="20" spans="4:4">
       <c r="B20" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C20" t="s">
         <v>40</v>
@@ -2247,7 +2387,23 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="4:4"/>
+    <row r="21" spans="4:4">
+      <c r="B21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C21" t="s">
+        <v>169</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" t="s">
+        <v>158</v>
+      </c>
+      <c r="F21" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="22" spans="4:4"/>
     <row r="23" spans="4:4"/>
     <row r="24" spans="4:4"/>

</xml_diff>

<commit_message>
Removed unused button from GUI
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17947" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18073" uniqueCount="191">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2162,7 +2162,7 @@
     </row>
     <row r="8" spans="2:10">
       <c r="B8" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="C8" t="s">
         <v>76</v>
@@ -2171,7 +2171,7 @@
         <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F8" t="s">
         <v>59</v>
@@ -2179,7 +2179,7 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C9" t="s">
         <v>76</v>
@@ -2188,7 +2188,7 @@
         <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="F9" t="s">
         <v>59</v>
@@ -2196,7 +2196,7 @@
     </row>
     <row r="10" spans="2:10">
       <c r="B10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C10" t="s">
         <v>76</v>
@@ -2205,7 +2205,7 @@
         <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F10" t="s">
         <v>59</v>
@@ -2213,7 +2213,7 @@
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C11" t="s">
         <v>76</v>
@@ -2222,7 +2222,7 @@
         <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="F11" t="s">
         <v>59</v>
@@ -2230,16 +2230,16 @@
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>137</v>
+        <v>95</v>
       </c>
       <c r="F12" t="s">
         <v>59</v>
@@ -2247,16 +2247,16 @@
     </row>
     <row r="13" spans="2:10">
       <c r="B13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
-        <v>95</v>
+        <v>155</v>
       </c>
       <c r="F13" t="s">
         <v>59</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="14" spans="2:10">
       <c r="B14" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C14" t="s">
         <v>76</v>
@@ -2273,7 +2273,7 @@
         <v>58</v>
       </c>
       <c r="E14" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="F14" t="s">
         <v>59</v>
@@ -2281,16 +2281,16 @@
     </row>
     <row r="15" spans="2:10">
       <c r="B15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C15" t="s">
         <v>76</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>144</v>
       </c>
       <c r="E15" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="F15" t="s">
         <v>59</v>
@@ -2298,16 +2298,16 @@
     </row>
     <row r="16" spans="2:10">
       <c r="B16" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="C16" t="s">
         <v>76</v>
       </c>
       <c r="D16" t="s">
-        <v>144</v>
+        <v>58</v>
       </c>
       <c r="E16" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="F16" t="s">
         <v>59</v>
@@ -2315,16 +2315,16 @@
     </row>
     <row r="17" spans="4:4">
       <c r="B17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E17" t="s">
-        <v>153</v>
+        <v>95</v>
       </c>
       <c r="F17" t="s">
         <v>59</v>
@@ -2332,78 +2332,62 @@
     </row>
     <row r="18" spans="4:4">
       <c r="B18" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>169</v>
       </c>
       <c r="D18" t="s">
         <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>95</v>
+        <v>189</v>
       </c>
       <c r="F18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="19" spans="4:4">
       <c r="B19" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s">
-        <v>169</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
         <v>62</v>
       </c>
       <c r="E19" t="s">
-        <v>189</v>
+        <v>95</v>
       </c>
       <c r="F19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19" t="s">
-        <v>62</v>
-      </c>
-      <c r="H19" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="20" spans="4:4">
       <c r="B20" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>169</v>
       </c>
       <c r="D20" t="s">
         <v>62</v>
       </c>
       <c r="E20" t="s">
-        <v>95</v>
+        <v>158</v>
       </c>
       <c r="F20" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="4:4">
-      <c r="B21" t="s">
-        <v>164</v>
-      </c>
-      <c r="C21" t="s">
-        <v>169</v>
-      </c>
-      <c r="D21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" t="s">
-        <v>158</v>
-      </c>
-      <c r="F21" t="s">
-        <v>59</v>
-      </c>
-    </row>
+    <row r="21" spans="4:4"/>
     <row r="22" spans="4:4"/>
     <row r="23" spans="4:4"/>
     <row r="24" spans="4:4"/>

</xml_diff>